<commit_message>
Saving some fake data
</commit_message>
<xml_diff>
--- a/Database Repository/EdusafeServicingDB Repository/0. Helper Scripts and Excel/Helper Workbook.xlsx
+++ b/Database Repository/EdusafeServicingDB Repository/0. Helper Scripts and Excel/Helper Workbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dar Vadar\Desktop\EduSafe Repo\edusafe\Database Repository\EdusafeServicingDB Repository\0. Helper Scripts and Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5AFE81B-A09B-44E0-8E68-43F5CA601DC7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21DE8306-3EA0-4778-88EC-54BA0380C023}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{4F07375E-5034-49E5-AD40-EDFCB413E4AD}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="265">
   <si>
     <t>Database</t>
   </si>
@@ -812,6 +812,39 @@
   </si>
   <si>
     <t>'Semester'</t>
+  </si>
+  <si>
+    <t>SP_DeleteEmails</t>
+  </si>
+  <si>
+    <t>SP_UpdateEmails</t>
+  </si>
+  <si>
+    <t>,1</t>
+  </si>
+  <si>
+    <t>1,'Matthew.Moore@Edusafe.com'</t>
+  </si>
+  <si>
+    <t>,0</t>
+  </si>
+  <si>
+    <t>1,'Matthew.Moore@gmail.com'</t>
+  </si>
+  <si>
+    <t>2,'Sharon.Paesachov@EduSafe.com'</t>
+  </si>
+  <si>
+    <t>2,'Sharon.Paesachov@gmail.com'</t>
+  </si>
+  <si>
+    <t>3,'Anomandaris.Dragnipurake@malazan.awesome'</t>
+  </si>
+  <si>
+    <t>4,'Butt.McPoopypants@poopooville.poopoo'</t>
+  </si>
+  <si>
+    <t>5,'Trull.Sengar@malazan.awesome'</t>
   </si>
 </sst>
 </file>
@@ -1925,10 +1958,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF7A6780-4CB8-4C87-9527-D541C7D9DA48}">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1953,7 +1986,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>254</v>
       </c>
       <c r="B2" t="s">
         <v>42</v>
@@ -1962,7 +1995,7 @@
         <v>83</v>
       </c>
       <c r="D2" t="str">
-        <f t="shared" ref="D2" si="0">"sqlcmd -S "
+        <f t="shared" ref="D2:D3" si="0">"sqlcmd -S "
 &amp;Entries_Server
 &amp;" -d "
 &amp;Entries_Database
@@ -1976,12 +2009,12 @@
 &amp;""""
 &amp;" &gt;&gt; """
 &amp;Entries_StoredProcedure_DebugText</f>
-        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\cust.SP_InsertEmails.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
+        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\cust.SP_DeleteEmails.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>255</v>
       </c>
       <c r="B3" t="s">
         <v>42</v>
@@ -1990,26 +2023,13 @@
         <v>83</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3" si="1">"sqlcmd -S "
-&amp;Entries_Server
-&amp;" -d "
-&amp;Entries_Database
-&amp;" -U "
-&amp;Entries_User
-&amp;" -P "
-&amp;Entries_Password
-&amp;" -i "
-&amp;Entries_StoredProcedure_RootPath
-&amp;B3&amp;A3&amp;C3
-&amp;""""
-&amp;" &gt;&gt; """
-&amp;Entries_StoredProcedure_DebugText</f>
-        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\cust.SP_InsertEmailsSet.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
+        <f t="shared" si="0"/>
+        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\cust.SP_UpdateEmails.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>95</v>
       </c>
       <c r="B4" t="s">
         <v>42</v>
@@ -2018,7 +2038,7 @@
         <v>83</v>
       </c>
       <c r="D4" t="str">
-        <f t="shared" ref="D4:D35" si="2">"sqlcmd -S "
+        <f t="shared" ref="D4" si="1">"sqlcmd -S "
 &amp;Entries_Server
 &amp;" -d "
 &amp;Entries_Database
@@ -2032,42 +2052,68 @@
 &amp;""""
 &amp;" &gt;&gt; """
 &amp;Entries_StoredProcedure_DebugText</f>
-        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\cust.SP_InsertInsureesAccountData.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
+        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\cust.SP_InsertEmails.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>93</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
         <v>83</v>
       </c>
       <c r="D5" t="str">
-        <f t="shared" si="2"/>
-        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertClaimAccountEntry.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
+        <f t="shared" ref="D5" si="2">"sqlcmd -S "
+&amp;Entries_Server
+&amp;" -d "
+&amp;Entries_Database
+&amp;" -U "
+&amp;Entries_User
+&amp;" -P "
+&amp;Entries_Password
+&amp;" -i "
+&amp;Entries_StoredProcedure_RootPath
+&amp;B5&amp;A5&amp;C5
+&amp;""""
+&amp;" &gt;&gt; """
+&amp;Entries_StoredProcedure_DebugText</f>
+        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\cust.SP_InsertEmailsSet.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
         <v>83</v>
       </c>
       <c r="D6" t="str">
-        <f t="shared" si="2"/>
-        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertClaimDocumentEntry.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
+        <f t="shared" ref="D6:D37" si="3">"sqlcmd -S "
+&amp;Entries_Server
+&amp;" -d "
+&amp;Entries_Database
+&amp;" -U "
+&amp;Entries_User
+&amp;" -P "
+&amp;Entries_Password
+&amp;" -i "
+&amp;Entries_StoredProcedure_RootPath
+&amp;B6&amp;A6&amp;C6
+&amp;""""
+&amp;" &gt;&gt; """
+&amp;Entries_StoredProcedure_DebugText</f>
+        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\cust.SP_InsertInsureesAccountData.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
         <v>22</v>
@@ -2076,13 +2122,13 @@
         <v>83</v>
       </c>
       <c r="D7" t="str">
-        <f t="shared" si="2"/>
-        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertClaimOptionEntry.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
+        <f t="shared" si="3"/>
+        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertClaimAccountEntry.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
         <v>22</v>
@@ -2091,13 +2137,13 @@
         <v>83</v>
       </c>
       <c r="D8" t="str">
-        <f t="shared" si="2"/>
-        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertClaimPaymentEntry.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
+        <f t="shared" si="3"/>
+        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertClaimDocumentEntry.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
         <v>22</v>
@@ -2106,13 +2152,13 @@
         <v>83</v>
       </c>
       <c r="D9" t="str">
-        <f t="shared" si="2"/>
-        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertClaimStatusEntry.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
+        <f t="shared" si="3"/>
+        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertClaimOptionEntry.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B10" t="s">
         <v>22</v>
@@ -2121,13 +2167,13 @@
         <v>83</v>
       </c>
       <c r="D10" t="str">
-        <f t="shared" si="2"/>
-        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertClaimStatusType.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
+        <f t="shared" si="3"/>
+        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertClaimPaymentEntry.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
         <v>22</v>
@@ -2136,13 +2182,13 @@
         <v>83</v>
       </c>
       <c r="D11" t="str">
-        <f t="shared" si="2"/>
-        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertCollegeAcademicTermType.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
+        <f t="shared" si="3"/>
+        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertClaimStatusEntry.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s">
         <v>22</v>
@@ -2151,13 +2197,13 @@
         <v>83</v>
       </c>
       <c r="D12" t="str">
-        <f t="shared" si="2"/>
-        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertCollegeDetail.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
+        <f t="shared" si="3"/>
+        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertClaimStatusType.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B13" t="s">
         <v>22</v>
@@ -2166,13 +2212,13 @@
         <v>83</v>
       </c>
       <c r="D13" t="str">
-        <f t="shared" si="2"/>
-        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertCollegeMajor.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
+        <f t="shared" si="3"/>
+        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertCollegeAcademicTermType.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B14" t="s">
         <v>22</v>
@@ -2181,13 +2227,13 @@
         <v>83</v>
       </c>
       <c r="D14" t="str">
-        <f t="shared" si="2"/>
-        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertCollegeType.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
+        <f t="shared" si="3"/>
+        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertCollegeDetail.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B15" t="s">
         <v>22</v>
@@ -2196,13 +2242,13 @@
         <v>83</v>
       </c>
       <c r="D15" t="str">
-        <f t="shared" si="2"/>
-        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertFileVerificationStatusType.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
+        <f t="shared" si="3"/>
+        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertCollegeMajor.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B16" t="s">
         <v>22</v>
@@ -2211,13 +2257,13 @@
         <v>83</v>
       </c>
       <c r="D16" t="str">
-        <f t="shared" si="2"/>
-        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertInstitutionsAccountData.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
+        <f t="shared" si="3"/>
+        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertCollegeType.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B17" t="s">
         <v>22</v>
@@ -2226,13 +2272,13 @@
         <v>83</v>
       </c>
       <c r="D17" t="str">
-        <f t="shared" si="2"/>
-        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertInstitutionsInsureeList.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
+        <f t="shared" si="3"/>
+        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertFileVerificationStatusType.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B18" t="s">
         <v>22</v>
@@ -2241,13 +2287,13 @@
         <v>83</v>
       </c>
       <c r="D18" t="str">
-        <f t="shared" si="2"/>
-        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertInstitutionsNextPaymentAndBalanceInformation.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
+        <f t="shared" si="3"/>
+        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertInstitutionsAccountData.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B19" t="s">
         <v>22</v>
@@ -2256,13 +2302,13 @@
         <v>83</v>
       </c>
       <c r="D19" t="str">
-        <f t="shared" si="2"/>
-        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertInstitutionsNotificationHistoryEntry.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
+        <f t="shared" si="3"/>
+        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertInstitutionsInsureeList.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B20" t="s">
         <v>22</v>
@@ -2271,13 +2317,13 @@
         <v>83</v>
       </c>
       <c r="D20" t="str">
-        <f t="shared" si="2"/>
-        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertInstitutionsPaymentHistoryEntry.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
+        <f t="shared" si="3"/>
+        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertInstitutionsNextPaymentAndBalanceInformation.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B21" t="s">
         <v>22</v>
@@ -2286,13 +2332,13 @@
         <v>83</v>
       </c>
       <c r="D21" t="str">
-        <f t="shared" si="2"/>
-        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertInsureesAcademicHistory.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
+        <f t="shared" si="3"/>
+        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertInstitutionsNotificationHistoryEntry.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B22" t="s">
         <v>22</v>
@@ -2301,13 +2347,13 @@
         <v>83</v>
       </c>
       <c r="D22" t="str">
-        <f t="shared" si="2"/>
-        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertInsureesEnrollmentVerificationDetails.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
+        <f t="shared" si="3"/>
+        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertInstitutionsPaymentHistoryEntry.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B23" t="s">
         <v>22</v>
@@ -2316,13 +2362,13 @@
         <v>83</v>
       </c>
       <c r="D23" t="str">
-        <f t="shared" si="2"/>
-        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertInsureesGraduationVerificationDetails.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
+        <f t="shared" si="3"/>
+        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertInsureesAcademicHistory.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="B24" t="s">
         <v>22</v>
@@ -2331,13 +2377,13 @@
         <v>83</v>
       </c>
       <c r="D24" t="str">
-        <f t="shared" si="2"/>
-        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertInsureesMajorMinorDetails.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
+        <f t="shared" si="3"/>
+        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertInsureesEnrollmentVerificationDetails.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="B25" t="s">
         <v>22</v>
@@ -2346,13 +2392,13 @@
         <v>83</v>
       </c>
       <c r="D25" t="str">
-        <f t="shared" si="2"/>
-        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertInsureesMajorMinorDetailsSet.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
+        <f t="shared" si="3"/>
+        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertInsureesGraduationVerificationDetails.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="B26" t="s">
         <v>22</v>
@@ -2361,13 +2407,13 @@
         <v>83</v>
       </c>
       <c r="D26" t="str">
-        <f t="shared" si="2"/>
-        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertInsureesNextPaymentAndBalanceInformation.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
+        <f t="shared" si="3"/>
+        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertInsureesMajorMinorDetails.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>74</v>
+        <v>92</v>
       </c>
       <c r="B27" t="s">
         <v>22</v>
@@ -2376,13 +2422,13 @@
         <v>83</v>
       </c>
       <c r="D27" t="str">
-        <f t="shared" si="2"/>
-        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertInsureesNotificationHistoryEntry.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
+        <f t="shared" si="3"/>
+        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertInsureesMajorMinorDetailsSet.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B28" t="s">
         <v>22</v>
@@ -2391,13 +2437,13 @@
         <v>83</v>
       </c>
       <c r="D28" t="str">
-        <f t="shared" si="2"/>
-        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertInsureesPaymentHistoryEntry.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
+        <f t="shared" si="3"/>
+        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertInsureesNextPaymentAndBalanceInformation.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B29" t="s">
         <v>22</v>
@@ -2406,13 +2452,13 @@
         <v>83</v>
       </c>
       <c r="D29" t="str">
-        <f t="shared" si="2"/>
-        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertInsureesPremiumCalculationDetails.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
+        <f t="shared" si="3"/>
+        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertInsureesNotificationHistoryEntry.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B30" t="s">
         <v>22</v>
@@ -2421,13 +2467,13 @@
         <v>83</v>
       </c>
       <c r="D30" t="str">
-        <f t="shared" si="2"/>
-        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertInsureesPremiumCalculationDetailsSet.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
+        <f t="shared" si="3"/>
+        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertInsureesPaymentHistoryEntry.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B31" t="s">
         <v>22</v>
@@ -2436,13 +2482,13 @@
         <v>83</v>
       </c>
       <c r="D31" t="str">
-        <f t="shared" si="2"/>
-        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertInsureesPremiumCalculationOptionDetails.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
+        <f t="shared" si="3"/>
+        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertInsureesPremiumCalculationDetails.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B32" t="s">
         <v>22</v>
@@ -2451,13 +2497,13 @@
         <v>83</v>
       </c>
       <c r="D32" t="str">
-        <f t="shared" si="2"/>
-        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertInsureesPremiumCalculationOptionDetailsSet.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
+        <f t="shared" si="3"/>
+        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertInsureesPremiumCalculationDetailsSet.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B33" t="s">
         <v>22</v>
@@ -2466,13 +2512,13 @@
         <v>83</v>
       </c>
       <c r="D33" t="str">
-        <f t="shared" si="2"/>
-        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertNotificationType.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
+        <f t="shared" si="3"/>
+        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertInsureesPremiumCalculationOptionDetails.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B34" t="s">
         <v>22</v>
@@ -2481,13 +2527,13 @@
         <v>83</v>
       </c>
       <c r="D34" t="str">
-        <f t="shared" si="2"/>
-        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertOptionType.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
+        <f t="shared" si="3"/>
+        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertInsureesPremiumCalculationOptionDetailsSet.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B35" t="s">
         <v>22</v>
@@ -2496,7 +2542,37 @@
         <v>83</v>
       </c>
       <c r="D35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertNotificationType.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>81</v>
+      </c>
+      <c r="B36" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36" t="s">
+        <v>83</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="3"/>
+        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertOptionType.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>82</v>
+      </c>
+      <c r="B37" t="s">
+        <v>22</v>
+      </c>
+      <c r="C37" t="s">
+        <v>83</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="3"/>
         <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\dbo.SP_InsertPaymentStatusType.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
       </c>
     </row>
@@ -2509,8 +2585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{746F0001-40B4-4DDF-A81A-84108DB4EF26}">
   <dimension ref="A1:C73"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C78" sqref="C78"/>
+    <sheetView topLeftCell="A32" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38:C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2937,6 +3013,30 @@
         <v>IF EXISTS (SELECT * FROM INFORMATION_SCHEMA.TABLES WHERE TABLE_NAME = 'PaymentStatusType') BEGIN DROP TABLE dbo.PaymentStatusType END</v>
       </c>
     </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>254</v>
+      </c>
+      <c r="B38" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" ref="C38:C39" si="3">"IF EXISTS (SELECT * FROM sys.objects WHERE Type = 'P' and Name = '" &amp;A38 &amp;"' ) BEGIN DROP PROCEDURE " &amp;B38 &amp;A38&amp;" END"</f>
+        <v>IF EXISTS (SELECT * FROM sys.objects WHERE Type = 'P' and Name = 'SP_DeleteEmails' ) BEGIN DROP PROCEDURE cust.SP_DeleteEmails END</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>255</v>
+      </c>
+      <c r="B39" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" si="3"/>
+        <v>IF EXISTS (SELECT * FROM sys.objects WHERE Type = 'P' and Name = 'SP_UpdateEmails' ) BEGIN DROP PROCEDURE cust.SP_UpdateEmails END</v>
+      </c>
+    </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>95</v>
@@ -2957,7 +3057,7 @@
         <v>42</v>
       </c>
       <c r="C41" t="str">
-        <f t="shared" ref="C41:C72" si="3">"IF EXISTS (SELECT * FROM sys.objects WHERE Type = 'P' and Name = '" &amp;A41 &amp;"' ) BEGIN DROP PROCEDURE " &amp;B41 &amp;A41&amp;" END"</f>
+        <f t="shared" ref="C41:C72" si="4">"IF EXISTS (SELECT * FROM sys.objects WHERE Type = 'P' and Name = '" &amp;A41 &amp;"' ) BEGIN DROP PROCEDURE " &amp;B41 &amp;A41&amp;" END"</f>
         <v>IF EXISTS (SELECT * FROM sys.objects WHERE Type = 'P' and Name = 'SP_InsertEmailsSet' ) BEGIN DROP PROCEDURE cust.SP_InsertEmailsSet END</v>
       </c>
     </row>
@@ -2969,7 +3069,7 @@
         <v>42</v>
       </c>
       <c r="C42" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>IF EXISTS (SELECT * FROM sys.objects WHERE Type = 'P' and Name = 'SP_InsertInsureesAccountData' ) BEGIN DROP PROCEDURE cust.SP_InsertInsureesAccountData END</v>
       </c>
     </row>
@@ -2981,7 +3081,7 @@
         <v>22</v>
       </c>
       <c r="C43" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>IF EXISTS (SELECT * FROM sys.objects WHERE Type = 'P' and Name = 'SP_InsertClaimAccountEntry' ) BEGIN DROP PROCEDURE dbo.SP_InsertClaimAccountEntry END</v>
       </c>
     </row>
@@ -2993,7 +3093,7 @@
         <v>22</v>
       </c>
       <c r="C44" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>IF EXISTS (SELECT * FROM sys.objects WHERE Type = 'P' and Name = 'SP_InsertClaimDocumentEntry' ) BEGIN DROP PROCEDURE dbo.SP_InsertClaimDocumentEntry END</v>
       </c>
     </row>
@@ -3005,7 +3105,7 @@
         <v>22</v>
       </c>
       <c r="C45" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>IF EXISTS (SELECT * FROM sys.objects WHERE Type = 'P' and Name = 'SP_InsertClaimOptionEntry' ) BEGIN DROP PROCEDURE dbo.SP_InsertClaimOptionEntry END</v>
       </c>
     </row>
@@ -3017,7 +3117,7 @@
         <v>22</v>
       </c>
       <c r="C46" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>IF EXISTS (SELECT * FROM sys.objects WHERE Type = 'P' and Name = 'SP_InsertClaimPaymentEntry' ) BEGIN DROP PROCEDURE dbo.SP_InsertClaimPaymentEntry END</v>
       </c>
     </row>
@@ -3029,7 +3129,7 @@
         <v>22</v>
       </c>
       <c r="C47" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>IF EXISTS (SELECT * FROM sys.objects WHERE Type = 'P' and Name = 'SP_InsertClaimStatusEntry' ) BEGIN DROP PROCEDURE dbo.SP_InsertClaimStatusEntry END</v>
       </c>
     </row>
@@ -3041,7 +3141,7 @@
         <v>22</v>
       </c>
       <c r="C48" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>IF EXISTS (SELECT * FROM sys.objects WHERE Type = 'P' and Name = 'SP_InsertClaimStatusType' ) BEGIN DROP PROCEDURE dbo.SP_InsertClaimStatusType END</v>
       </c>
     </row>
@@ -3053,7 +3153,7 @@
         <v>22</v>
       </c>
       <c r="C49" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>IF EXISTS (SELECT * FROM sys.objects WHERE Type = 'P' and Name = 'SP_InsertCollegeAcademicTermType' ) BEGIN DROP PROCEDURE dbo.SP_InsertCollegeAcademicTermType END</v>
       </c>
     </row>
@@ -3065,7 +3165,7 @@
         <v>22</v>
       </c>
       <c r="C50" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>IF EXISTS (SELECT * FROM sys.objects WHERE Type = 'P' and Name = 'SP_InsertCollegeDetail' ) BEGIN DROP PROCEDURE dbo.SP_InsertCollegeDetail END</v>
       </c>
     </row>
@@ -3077,7 +3177,7 @@
         <v>22</v>
       </c>
       <c r="C51" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>IF EXISTS (SELECT * FROM sys.objects WHERE Type = 'P' and Name = 'SP_InsertCollegeMajor' ) BEGIN DROP PROCEDURE dbo.SP_InsertCollegeMajor END</v>
       </c>
     </row>
@@ -3089,7 +3189,7 @@
         <v>22</v>
       </c>
       <c r="C52" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>IF EXISTS (SELECT * FROM sys.objects WHERE Type = 'P' and Name = 'SP_InsertCollegeType' ) BEGIN DROP PROCEDURE dbo.SP_InsertCollegeType END</v>
       </c>
     </row>
@@ -3101,7 +3201,7 @@
         <v>22</v>
       </c>
       <c r="C53" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>IF EXISTS (SELECT * FROM sys.objects WHERE Type = 'P' and Name = 'SP_InsertFileVerificationStatusType' ) BEGIN DROP PROCEDURE dbo.SP_InsertFileVerificationStatusType END</v>
       </c>
     </row>
@@ -3113,7 +3213,7 @@
         <v>22</v>
       </c>
       <c r="C54" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>IF EXISTS (SELECT * FROM sys.objects WHERE Type = 'P' and Name = 'SP_InsertInstitutionsAccountData' ) BEGIN DROP PROCEDURE dbo.SP_InsertInstitutionsAccountData END</v>
       </c>
     </row>
@@ -3125,7 +3225,7 @@
         <v>22</v>
       </c>
       <c r="C55" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>IF EXISTS (SELECT * FROM sys.objects WHERE Type = 'P' and Name = 'SP_InsertInstitutionsInsureeList' ) BEGIN DROP PROCEDURE dbo.SP_InsertInstitutionsInsureeList END</v>
       </c>
     </row>
@@ -3137,7 +3237,7 @@
         <v>22</v>
       </c>
       <c r="C56" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>IF EXISTS (SELECT * FROM sys.objects WHERE Type = 'P' and Name = 'SP_InsertInstitutionsNextPaymentAndBalanceInformation' ) BEGIN DROP PROCEDURE dbo.SP_InsertInstitutionsNextPaymentAndBalanceInformation END</v>
       </c>
     </row>
@@ -3149,7 +3249,7 @@
         <v>22</v>
       </c>
       <c r="C57" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>IF EXISTS (SELECT * FROM sys.objects WHERE Type = 'P' and Name = 'SP_InsertInstitutionsNotificationHistoryEntry' ) BEGIN DROP PROCEDURE dbo.SP_InsertInstitutionsNotificationHistoryEntry END</v>
       </c>
     </row>
@@ -3161,7 +3261,7 @@
         <v>22</v>
       </c>
       <c r="C58" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>IF EXISTS (SELECT * FROM sys.objects WHERE Type = 'P' and Name = 'SP_InsertInstitutionsPaymentHistoryEntry' ) BEGIN DROP PROCEDURE dbo.SP_InsertInstitutionsPaymentHistoryEntry END</v>
       </c>
     </row>
@@ -3173,7 +3273,7 @@
         <v>22</v>
       </c>
       <c r="C59" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>IF EXISTS (SELECT * FROM sys.objects WHERE Type = 'P' and Name = 'SP_InsertInsureesAcademicHistory' ) BEGIN DROP PROCEDURE dbo.SP_InsertInsureesAcademicHistory END</v>
       </c>
     </row>
@@ -3185,7 +3285,7 @@
         <v>22</v>
       </c>
       <c r="C60" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>IF EXISTS (SELECT * FROM sys.objects WHERE Type = 'P' and Name = 'SP_InsertInsureesEnrollmentVerificationDetails' ) BEGIN DROP PROCEDURE dbo.SP_InsertInsureesEnrollmentVerificationDetails END</v>
       </c>
     </row>
@@ -3197,7 +3297,7 @@
         <v>22</v>
       </c>
       <c r="C61" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>IF EXISTS (SELECT * FROM sys.objects WHERE Type = 'P' and Name = 'SP_InsertInsureesGraduationVerificationDetails' ) BEGIN DROP PROCEDURE dbo.SP_InsertInsureesGraduationVerificationDetails END</v>
       </c>
     </row>
@@ -3209,7 +3309,7 @@
         <v>22</v>
       </c>
       <c r="C62" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>IF EXISTS (SELECT * FROM sys.objects WHERE Type = 'P' and Name = 'SP_InsertInsureesMajorMinorDetails' ) BEGIN DROP PROCEDURE dbo.SP_InsertInsureesMajorMinorDetails END</v>
       </c>
     </row>
@@ -3221,7 +3321,7 @@
         <v>22</v>
       </c>
       <c r="C63" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>IF EXISTS (SELECT * FROM sys.objects WHERE Type = 'P' and Name = 'SP_InsertInsureesMajorMinorDetailsSet' ) BEGIN DROP PROCEDURE dbo.SP_InsertInsureesMajorMinorDetailsSet END</v>
       </c>
     </row>
@@ -3233,7 +3333,7 @@
         <v>22</v>
       </c>
       <c r="C64" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>IF EXISTS (SELECT * FROM sys.objects WHERE Type = 'P' and Name = 'SP_InsertInsureesNextPaymentAndBalanceInformation' ) BEGIN DROP PROCEDURE dbo.SP_InsertInsureesNextPaymentAndBalanceInformation END</v>
       </c>
     </row>
@@ -3245,7 +3345,7 @@
         <v>22</v>
       </c>
       <c r="C65" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>IF EXISTS (SELECT * FROM sys.objects WHERE Type = 'P' and Name = 'SP_InsertInsureesNotificationHistoryEntry' ) BEGIN DROP PROCEDURE dbo.SP_InsertInsureesNotificationHistoryEntry END</v>
       </c>
     </row>
@@ -3257,7 +3357,7 @@
         <v>22</v>
       </c>
       <c r="C66" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>IF EXISTS (SELECT * FROM sys.objects WHERE Type = 'P' and Name = 'SP_InsertInsureesPaymentHistoryEntry' ) BEGIN DROP PROCEDURE dbo.SP_InsertInsureesPaymentHistoryEntry END</v>
       </c>
     </row>
@@ -3269,7 +3369,7 @@
         <v>22</v>
       </c>
       <c r="C67" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>IF EXISTS (SELECT * FROM sys.objects WHERE Type = 'P' and Name = 'SP_InsertInsureesPremiumCalculationDetails' ) BEGIN DROP PROCEDURE dbo.SP_InsertInsureesPremiumCalculationDetails END</v>
       </c>
     </row>
@@ -3281,7 +3381,7 @@
         <v>22</v>
       </c>
       <c r="C68" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>IF EXISTS (SELECT * FROM sys.objects WHERE Type = 'P' and Name = 'SP_InsertInsureesPremiumCalculationDetailsSet' ) BEGIN DROP PROCEDURE dbo.SP_InsertInsureesPremiumCalculationDetailsSet END</v>
       </c>
     </row>
@@ -3293,7 +3393,7 @@
         <v>22</v>
       </c>
       <c r="C69" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>IF EXISTS (SELECT * FROM sys.objects WHERE Type = 'P' and Name = 'SP_InsertInsureesPremiumCalculationOptionDetails' ) BEGIN DROP PROCEDURE dbo.SP_InsertInsureesPremiumCalculationOptionDetails END</v>
       </c>
     </row>
@@ -3305,7 +3405,7 @@
         <v>22</v>
       </c>
       <c r="C70" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>IF EXISTS (SELECT * FROM sys.objects WHERE Type = 'P' and Name = 'SP_InsertInsureesPremiumCalculationOptionDetailsSet' ) BEGIN DROP PROCEDURE dbo.SP_InsertInsureesPremiumCalculationOptionDetailsSet END</v>
       </c>
     </row>
@@ -3317,7 +3417,7 @@
         <v>22</v>
       </c>
       <c r="C71" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>IF EXISTS (SELECT * FROM sys.objects WHERE Type = 'P' and Name = 'SP_InsertNotificationType' ) BEGIN DROP PROCEDURE dbo.SP_InsertNotificationType END</v>
       </c>
     </row>
@@ -3329,7 +3429,7 @@
         <v>22</v>
       </c>
       <c r="C72" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>IF EXISTS (SELECT * FROM sys.objects WHERE Type = 'P' and Name = 'SP_InsertOptionType' ) BEGIN DROP PROCEDURE dbo.SP_InsertOptionType END</v>
       </c>
     </row>
@@ -3341,7 +3441,7 @@
         <v>22</v>
       </c>
       <c r="C73" t="str">
-        <f t="shared" ref="C73" si="4">"IF EXISTS (SELECT * FROM sys.objects WHERE Type = 'P' and Name = '" &amp;A73 &amp;"' ) BEGIN DROP PROCEDURE " &amp;B73 &amp;A73&amp;" END"</f>
+        <f t="shared" ref="C73" si="5">"IF EXISTS (SELECT * FROM sys.objects WHERE Type = 'P' and Name = '" &amp;A73 &amp;"' ) BEGIN DROP PROCEDURE " &amp;B73 &amp;A73&amp;" END"</f>
         <v>IF EXISTS (SELECT * FROM sys.objects WHERE Type = 'P' and Name = 'SP_InsertPaymentStatusType' ) BEGIN DROP PROCEDURE dbo.SP_InsertPaymentStatusType END</v>
       </c>
     </row>
@@ -3364,10 +3464,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED49A165-DA0E-484E-A56A-F98E21190960}">
-  <dimension ref="A1:P48"/>
+  <dimension ref="A1:P55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4586,13 +4686,19 @@
       <c r="B28" t="s">
         <v>207</v>
       </c>
+      <c r="C28" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>206</v>
       </c>
       <c r="B29" t="s">
-        <v>208</v>
+        <v>257</v>
+      </c>
+      <c r="C29" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
@@ -4600,7 +4706,10 @@
         <v>206</v>
       </c>
       <c r="B30" t="s">
-        <v>209</v>
+        <v>259</v>
+      </c>
+      <c r="C30" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
@@ -4608,7 +4717,10 @@
         <v>206</v>
       </c>
       <c r="B31" t="s">
-        <v>210</v>
+        <v>208</v>
+      </c>
+      <c r="C31" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
@@ -4616,135 +4728,263 @@
         <v>206</v>
       </c>
       <c r="B32" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+      <c r="C32" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>206</v>
       </c>
       <c r="B33" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+      <c r="C33" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>206</v>
       </c>
       <c r="B34" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+      <c r="C34" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>206</v>
       </c>
       <c r="B35" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+      <c r="C35" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>206</v>
       </c>
       <c r="B36" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+      <c r="C36" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>206</v>
       </c>
       <c r="B37" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+        <v>263</v>
+      </c>
+      <c r="C37" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>206</v>
       </c>
       <c r="B38" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+      <c r="C38" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>206</v>
       </c>
       <c r="B39" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+      <c r="C39" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>206</v>
       </c>
       <c r="B40" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="C40" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>206</v>
       </c>
       <c r="B41" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+      <c r="C41" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>206</v>
       </c>
       <c r="B42" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+      <c r="C42" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>206</v>
       </c>
       <c r="B43" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+      <c r="C43" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>206</v>
       </c>
       <c r="B44" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+      <c r="C44" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>206</v>
       </c>
       <c r="B45" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+      <c r="C45" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>206</v>
       </c>
       <c r="B46" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+      <c r="C46" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>206</v>
       </c>
       <c r="B47" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+      <c r="C47" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>206</v>
       </c>
       <c r="B48" t="s">
+        <v>220</v>
+      </c>
+      <c r="C48" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>206</v>
+      </c>
+      <c r="B49" t="s">
+        <v>221</v>
+      </c>
+      <c r="C49" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>206</v>
+      </c>
+      <c r="B50" t="s">
+        <v>222</v>
+      </c>
+      <c r="C50" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>206</v>
+      </c>
+      <c r="B51" t="s">
+        <v>223</v>
+      </c>
+      <c r="C51" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>206</v>
+      </c>
+      <c r="B52" t="s">
+        <v>224</v>
+      </c>
+      <c r="C52" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>206</v>
+      </c>
+      <c r="B53" t="s">
+        <v>225</v>
+      </c>
+      <c r="C53" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>206</v>
+      </c>
+      <c r="B54" t="s">
+        <v>226</v>
+      </c>
+      <c r="C54" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>206</v>
+      </c>
+      <c r="B55" t="s">
         <v>227</v>
+      </c>
+      <c r="C55" t="s">
+        <v>256</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update to schema with most of the fake data inserts
</commit_message>
<xml_diff>
--- a/Database Repository/EdusafeServicingDB Repository/0. Helper Scripts and Excel/Helper Workbook.xlsx
+++ b/Database Repository/EdusafeServicingDB Repository/0. Helper Scripts and Excel/Helper Workbook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dar Vadar\Desktop\EduSafe Repo\edusafe\Database Repository\EdusafeServicingDB Repository\0. Helper Scripts and Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21DE8306-3EA0-4778-88EC-54BA0380C023}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{645275E1-67CD-42C8-BC59-BBBC54C842AE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{4F07375E-5034-49E5-AD40-EDFCB413E4AD}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4F07375E-5034-49E5-AD40-EDFCB413E4AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Entries" sheetId="2" r:id="rId1"/>
@@ -18,8 +18,6 @@
     <sheet name="Store Procs" sheetId="4" r:id="rId3"/>
     <sheet name="Rollback" sheetId="3" r:id="rId4"/>
     <sheet name="Inserts &gt;&gt;" sheetId="6" r:id="rId5"/>
-    <sheet name="cust. tables" sheetId="5" r:id="rId6"/>
-    <sheet name="college inserts" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tables!$A$1:$D$1</definedName>
@@ -50,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="102">
   <si>
     <t>Database</t>
   </si>
@@ -316,9 +314,6 @@
     <t>CreateSp.txt</t>
   </si>
   <si>
-    <t>6. Constraints</t>
-  </si>
-  <si>
     <t>.Constraints.sql</t>
   </si>
   <si>
@@ -340,405 +335,6 @@
     <t>SP_InsertEmails</t>
   </si>
   <si>
-    <t>@FolderPath</t>
-  </si>
-  <si>
-    <t>varchar</t>
-  </si>
-  <si>
-    <t>@FirstName</t>
-  </si>
-  <si>
-    <t>@MiddleName</t>
-  </si>
-  <si>
-    <t>@LastName</t>
-  </si>
-  <si>
-    <t>@SSN</t>
-  </si>
-  <si>
-    <t>bigint</t>
-  </si>
-  <si>
-    <t>@Birthdate</t>
-  </si>
-  <si>
-    <t>datetime</t>
-  </si>
-  <si>
-    <t>@Address1</t>
-  </si>
-  <si>
-    <t>@Address2</t>
-  </si>
-  <si>
-    <t>@Address3</t>
-  </si>
-  <si>
-    <t>@City</t>
-  </si>
-  <si>
-    <t>@State</t>
-  </si>
-  <si>
-    <t>@Zipcode</t>
-  </si>
-  <si>
-    <t>@IsInsuredViaInstitution</t>
-  </si>
-  <si>
-    <t>bit</t>
-  </si>
-  <si>
-    <t>NULL</t>
-  </si>
-  <si>
-    <t>Entry</t>
-  </si>
-  <si>
-    <t>nullable</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Matthew</t>
-  </si>
-  <si>
-    <t>Michaels</t>
-  </si>
-  <si>
-    <t>Moore</t>
-  </si>
-  <si>
-    <t>123 Awesome street</t>
-  </si>
-  <si>
-    <t>Anytown</t>
-  </si>
-  <si>
-    <t>124 Awesome street</t>
-  </si>
-  <si>
-    <t>125 Awesome street</t>
-  </si>
-  <si>
-    <t>126 Awesome street</t>
-  </si>
-  <si>
-    <t>127 Awesome street</t>
-  </si>
-  <si>
-    <t>128 Awesome street</t>
-  </si>
-  <si>
-    <t>129 Awesome street</t>
-  </si>
-  <si>
-    <t>130 Awesome street</t>
-  </si>
-  <si>
-    <t>131 Awesome street</t>
-  </si>
-  <si>
-    <t>132 Awesome street</t>
-  </si>
-  <si>
-    <t>133 Awesome street</t>
-  </si>
-  <si>
-    <t>134 Awesome street</t>
-  </si>
-  <si>
-    <t>135 Awesome street</t>
-  </si>
-  <si>
-    <t>136 Awesome street</t>
-  </si>
-  <si>
-    <t>137 Awesome street</t>
-  </si>
-  <si>
-    <t>138 Awesome street</t>
-  </si>
-  <si>
-    <t>139 Awesome street</t>
-  </si>
-  <si>
-    <t>140 Awesome street</t>
-  </si>
-  <si>
-    <t>141 Awesome street</t>
-  </si>
-  <si>
-    <t>142 Awesome street</t>
-  </si>
-  <si>
-    <t>143 Awesome street</t>
-  </si>
-  <si>
-    <t>Sharon</t>
-  </si>
-  <si>
-    <t>Paesachov</t>
-  </si>
-  <si>
-    <t>Dragnipurake</t>
-  </si>
-  <si>
-    <t>Anomandaris</t>
-  </si>
-  <si>
-    <t>Butt</t>
-  </si>
-  <si>
-    <t>Face</t>
-  </si>
-  <si>
-    <t>McPoopypants</t>
-  </si>
-  <si>
-    <t>Trull</t>
-  </si>
-  <si>
-    <t>Sengar</t>
-  </si>
-  <si>
-    <t>Paul</t>
-  </si>
-  <si>
-    <t>Atreides</t>
-  </si>
-  <si>
-    <t>Karsa</t>
-  </si>
-  <si>
-    <t>Orlong</t>
-  </si>
-  <si>
-    <t>Whiskey</t>
-  </si>
-  <si>
-    <t>Jack</t>
-  </si>
-  <si>
-    <t>Fiddler</t>
-  </si>
-  <si>
-    <t>Strings</t>
-  </si>
-  <si>
-    <t>Superman</t>
-  </si>
-  <si>
-    <t>Clark</t>
-  </si>
-  <si>
-    <t>Kent</t>
-  </si>
-  <si>
-    <t>Bruce</t>
-  </si>
-  <si>
-    <t>Batman</t>
-  </si>
-  <si>
-    <t>Wayne</t>
-  </si>
-  <si>
-    <t>Dassem</t>
-  </si>
-  <si>
-    <t>Ultor</t>
-  </si>
-  <si>
-    <t>Onos</t>
-  </si>
-  <si>
-    <t>T'oolan</t>
-  </si>
-  <si>
-    <t>FirstSword</t>
-  </si>
-  <si>
-    <t>Kalam</t>
-  </si>
-  <si>
-    <t>Mekhar</t>
-  </si>
-  <si>
-    <t>Eye</t>
-  </si>
-  <si>
-    <t>See</t>
-  </si>
-  <si>
-    <t>Youpee</t>
-  </si>
-  <si>
-    <t>Elephant</t>
-  </si>
-  <si>
-    <t>Shoe</t>
-  </si>
-  <si>
-    <t>Kurt</t>
-  </si>
-  <si>
-    <t>Vonnegut</t>
-  </si>
-  <si>
-    <t>Muad</t>
-  </si>
-  <si>
-    <t>Dib</t>
-  </si>
-  <si>
-    <t>Mario</t>
-  </si>
-  <si>
-    <t>And</t>
-  </si>
-  <si>
-    <t>Luigi</t>
-  </si>
-  <si>
-    <t>Princess</t>
-  </si>
-  <si>
-    <t>Peach</t>
-  </si>
-  <si>
-    <t xml:space="preserve">King </t>
-  </si>
-  <si>
-    <t>Koopa</t>
-  </si>
-  <si>
-    <t>Kurald Galain</t>
-  </si>
-  <si>
-    <t>Poopsville</t>
-  </si>
-  <si>
-    <t>CA</t>
-  </si>
-  <si>
-    <t>NV</t>
-  </si>
-  <si>
-    <t>Kurald Emurhlan</t>
-  </si>
-  <si>
-    <t>Dune</t>
-  </si>
-  <si>
-    <t>Teblor</t>
-  </si>
-  <si>
-    <t>Malazan</t>
-  </si>
-  <si>
-    <t>Smallville</t>
-  </si>
-  <si>
-    <t>IO</t>
-  </si>
-  <si>
-    <t>Gotham City</t>
-  </si>
-  <si>
-    <t>NY</t>
-  </si>
-  <si>
-    <t>Clanless</t>
-  </si>
-  <si>
-    <t>Somewhere Gross</t>
-  </si>
-  <si>
-    <t>La Zoo</t>
-  </si>
-  <si>
-    <t>Caladan</t>
-  </si>
-  <si>
-    <t>Nintendo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXEC cust.SP_InsertInsureesAccountData </t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXEC cust.SP_InsertEmails </t>
-  </si>
-  <si>
-    <t>1,'Matthew.Moore@soWhatWhoCares.com'</t>
-  </si>
-  <si>
-    <t>2,'Sharon.Paesachov@soWhatWhoCares.com'</t>
-  </si>
-  <si>
-    <t>3,'Anomandaris.Dragnipurake@soWhatWhoCares.com'</t>
-  </si>
-  <si>
-    <t>4,'Butt.McPoopypants@soWhatWhoCares.com'</t>
-  </si>
-  <si>
-    <t>5,'Trull.Sengar@soWhatWhoCares.com'</t>
-  </si>
-  <si>
-    <t>6,'Paul.Atreides@soWhatWhoCares.com'</t>
-  </si>
-  <si>
-    <t>7,'Karsa.Orlong@soWhatWhoCares.com'</t>
-  </si>
-  <si>
-    <t>8,'Whiskey.Jack@soWhatWhoCares.com'</t>
-  </si>
-  <si>
-    <t>9,'Fiddler.Strings@soWhatWhoCares.com'</t>
-  </si>
-  <si>
-    <t>10,'Clark.Kent@soWhatWhoCares.com'</t>
-  </si>
-  <si>
-    <t>11,'Bruce.Wayne@soWhatWhoCares.com'</t>
-  </si>
-  <si>
-    <t>12,'Dassem.Ultor@soWhatWhoCares.com'</t>
-  </si>
-  <si>
-    <t>13,'Onos.T'oolan@soWhatWhoCares.com'</t>
-  </si>
-  <si>
-    <t>14,'Kalam.Mekhar@soWhatWhoCares.com'</t>
-  </si>
-  <si>
-    <t>15,'Eye.Youpee@soWhatWhoCares.com'</t>
-  </si>
-  <si>
-    <t>16,'Elephant.Shoe@soWhatWhoCares.com'</t>
-  </si>
-  <si>
-    <t>17,'Kurt.Vonnegut@soWhatWhoCares.com'</t>
-  </si>
-  <si>
-    <t>18,'Muad.Dib@soWhatWhoCares.com'</t>
-  </si>
-  <si>
-    <t>19,'Mario.Luigi@soWhatWhoCares.com'</t>
-  </si>
-  <si>
-    <t>20,'Princess.Peach@soWhatWhoCares.com'</t>
-  </si>
-  <si>
-    <t>21,'King .Koopa@soWhatWhoCares.com'</t>
-  </si>
-  <si>
-    <t>dbo.ForeignKeyConstraints</t>
-  </si>
-  <si>
     <t>Constraints Root Path</t>
   </si>
   <si>
@@ -748,118 +344,26 @@
     <t>CreateFK.txt</t>
   </si>
   <si>
-    <t>Id</t>
-  </si>
-  <si>
-    <t>int</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>CreatedOn</t>
-  </si>
-  <si>
-    <t>CreatedBy</t>
-  </si>
-  <si>
-    <t>CollegeName</t>
-  </si>
-  <si>
-    <t>CollegeTypeId</t>
-  </si>
-  <si>
-    <t>CollegeAcademicTermTypeId</t>
-  </si>
-  <si>
-    <t>Public</t>
-  </si>
-  <si>
-    <t>Public Institutions</t>
-  </si>
-  <si>
-    <t>Private</t>
-  </si>
-  <si>
-    <t>Private Institutions</t>
-  </si>
-  <si>
-    <t>ForProfit</t>
-  </si>
-  <si>
-    <t>For-Profit Institutions</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Semester</t>
-  </si>
-  <si>
-    <t>Quarter</t>
-  </si>
-  <si>
-    <t>Trimester</t>
-  </si>
-  <si>
-    <t>EXEC InsertCollegeDetail</t>
-  </si>
-  <si>
-    <t>'AnyCollegeUSA',</t>
-  </si>
-  <si>
-    <t>'ForProfit',</t>
-  </si>
-  <si>
-    <t>'Semester'</t>
-  </si>
-  <si>
     <t>SP_DeleteEmails</t>
   </si>
   <si>
     <t>SP_UpdateEmails</t>
   </si>
   <si>
-    <t>,1</t>
-  </si>
-  <si>
-    <t>1,'Matthew.Moore@Edusafe.com'</t>
-  </si>
-  <si>
-    <t>,0</t>
-  </si>
-  <si>
-    <t>1,'Matthew.Moore@gmail.com'</t>
-  </si>
-  <si>
-    <t>2,'Sharon.Paesachov@EduSafe.com'</t>
-  </si>
-  <si>
-    <t>2,'Sharon.Paesachov@gmail.com'</t>
-  </si>
-  <si>
-    <t>3,'Anomandaris.Dragnipurake@malazan.awesome'</t>
-  </si>
-  <si>
-    <t>4,'Butt.McPoopypants@poopooville.poopoo'</t>
-  </si>
-  <si>
-    <t>5,'Trull.Sengar@malazan.awesome'</t>
+    <t>ForeignKeyConstraints</t>
+  </si>
+  <si>
+    <t>"6. Constraints\</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri Light"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri Light"/>
       <family val="2"/>
     </font>
@@ -884,10 +388,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1205,7 +707,7 @@
   <dimension ref="B2:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1283,18 +785,18 @@
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>229</v>
+        <v>95</v>
       </c>
       <c r="C11" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>230</v>
+        <v>96</v>
       </c>
       <c r="C12" t="s">
-        <v>231</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1306,7 +808,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D6E4056-ECB1-45E1-9DAC-970AA7C8F4F6}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
@@ -1332,7 +834,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
         <v>42</v>
@@ -1360,7 +862,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B3" t="s">
         <v>42</v>
@@ -1920,13 +1422,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>228</v>
+        <v>100</v>
       </c>
       <c r="B38" t="s">
         <v>22</v>
       </c>
       <c r="C38" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D38" t="str">
         <f>"sqlcmd -S "
@@ -1943,7 +1445,7 @@
 &amp;""""
 &amp;" &gt;&gt; """
 &amp;Entries_Constraints_Debug_Text</f>
-        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i 6. Constraintsdbo.dbo.ForeignKeyConstraints.Constraints.sql" &gt;&gt; "CreateFK.txt</v>
+        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "6. Constraints\dbo.ForeignKeyConstraints.Constraints.sql" &gt;&gt; "CreateFK.txt</v>
       </c>
     </row>
   </sheetData>
@@ -1960,8 +1462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF7A6780-4CB8-4C87-9527-D541C7D9DA48}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1986,7 +1488,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>254</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
         <v>42</v>
@@ -2014,7 +1516,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>255</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
         <v>42</v>
@@ -2029,7 +1531,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B4" t="s">
         <v>42</v>
@@ -2057,7 +1559,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B5" t="s">
         <v>42</v>
@@ -2398,7 +1900,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B26" t="s">
         <v>22</v>
@@ -2413,7 +1915,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B27" t="s">
         <v>22</v>
@@ -2585,7 +2087,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{746F0001-40B4-4DDF-A81A-84108DB4EF26}">
   <dimension ref="A1:C73"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView topLeftCell="A50" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C38" sqref="C38:C39"/>
     </sheetView>
   </sheetViews>
@@ -2607,7 +2109,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
         <v>42</v>
@@ -2619,7 +2121,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B3" t="s">
         <v>42</v>
@@ -3015,7 +2517,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>254</v>
+        <v>98</v>
       </c>
       <c r="B38" t="s">
         <v>42</v>
@@ -3027,7 +2529,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>255</v>
+        <v>99</v>
       </c>
       <c r="B39" t="s">
         <v>42</v>
@@ -3039,7 +2541,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B40" t="s">
         <v>42</v>
@@ -3051,7 +2553,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B41" t="s">
         <v>42</v>
@@ -3303,7 +2805,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B62" t="s">
         <v>22</v>
@@ -3315,7 +2817,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B63" t="s">
         <v>22</v>
@@ -3460,1797 +2962,4 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED49A165-DA0E-484E-A56A-F98E21190960}">
-  <dimension ref="A1:P55"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="O32" sqref="O32"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.75" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G1" t="s">
-        <v>103</v>
-      </c>
-      <c r="H1" t="s">
-        <v>105</v>
-      </c>
-      <c r="I1" t="s">
-        <v>106</v>
-      </c>
-      <c r="J1" t="s">
-        <v>107</v>
-      </c>
-      <c r="K1" t="s">
-        <v>108</v>
-      </c>
-      <c r="L1" t="s">
-        <v>109</v>
-      </c>
-      <c r="M1" t="s">
-        <v>110</v>
-      </c>
-      <c r="N1" t="s">
-        <v>111</v>
-      </c>
-      <c r="P1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D2" t="s">
-        <v>97</v>
-      </c>
-      <c r="E2" t="s">
-        <v>97</v>
-      </c>
-      <c r="F2" t="s">
-        <v>102</v>
-      </c>
-      <c r="G2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I2" t="s">
-        <v>97</v>
-      </c>
-      <c r="J2" t="s">
-        <v>97</v>
-      </c>
-      <c r="K2" t="s">
-        <v>97</v>
-      </c>
-      <c r="L2" t="s">
-        <v>97</v>
-      </c>
-      <c r="M2" t="s">
-        <v>97</v>
-      </c>
-      <c r="N2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B3">
-        <v>250</v>
-      </c>
-      <c r="C3">
-        <v>25</v>
-      </c>
-      <c r="D3">
-        <v>25</v>
-      </c>
-      <c r="E3">
-        <v>25</v>
-      </c>
-      <c r="F3">
-        <v>8</v>
-      </c>
-      <c r="G3">
-        <v>8</v>
-      </c>
-      <c r="H3">
-        <v>50</v>
-      </c>
-      <c r="I3">
-        <v>50</v>
-      </c>
-      <c r="J3">
-        <v>50</v>
-      </c>
-      <c r="K3">
-        <v>50</v>
-      </c>
-      <c r="L3">
-        <v>2</v>
-      </c>
-      <c r="M3">
-        <v>5</v>
-      </c>
-      <c r="N3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>114</v>
-      </c>
-      <c r="B4" t="s">
-        <v>115</v>
-      </c>
-      <c r="D4" t="s">
-        <v>115</v>
-      </c>
-      <c r="F4" t="s">
-        <v>116</v>
-      </c>
-      <c r="G4" t="s">
-        <v>116</v>
-      </c>
-      <c r="H4" t="s">
-        <v>116</v>
-      </c>
-      <c r="I4" t="s">
-        <v>115</v>
-      </c>
-      <c r="J4" t="s">
-        <v>115</v>
-      </c>
-      <c r="K4" t="s">
-        <v>116</v>
-      </c>
-      <c r="L4" t="s">
-        <v>116</v>
-      </c>
-      <c r="M4" t="s">
-        <v>116</v>
-      </c>
-      <c r="N4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C5" t="s">
-        <v>117</v>
-      </c>
-      <c r="D5" t="s">
-        <v>118</v>
-      </c>
-      <c r="E5" t="s">
-        <v>119</v>
-      </c>
-      <c r="F5">
-        <v>123456789</v>
-      </c>
-      <c r="G5" s="1">
-        <v>1</v>
-      </c>
-      <c r="H5" t="s">
-        <v>120</v>
-      </c>
-      <c r="I5" t="s">
-        <v>113</v>
-      </c>
-      <c r="J5" t="s">
-        <v>113</v>
-      </c>
-      <c r="K5" t="s">
-        <v>121</v>
-      </c>
-      <c r="L5" t="s">
-        <v>190</v>
-      </c>
-      <c r="M5">
-        <v>99999</v>
-      </c>
-      <c r="N5">
-        <v>1</v>
-      </c>
-      <c r="P5" t="str">
-        <f>$P$1&amp;B5&amp;",'"&amp;C5&amp;"',"&amp;IF(D5="NULL","NULL,","'"&amp;D5&amp;"','")&amp;E5&amp;"',"&amp;F5&amp;",'"&amp;TEXT(G5,("yyyy-mm-dd"))&amp;"','"&amp;H5&amp;"',"&amp;I5&amp;","&amp;J5&amp;",'"&amp;K5&amp;"','"&amp;L5&amp;"','"&amp;M5&amp;"',"&amp;N5</f>
-        <v>EXEC cust.SP_InsertInsureesAccountData NULL,'Matthew','Michaels','Moore',123456789,'1900-01-01','123 Awesome street',NULL,NULL,'Anytown','CA','99999',1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <f>A5+1</f>
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>113</v>
-      </c>
-      <c r="C6" t="s">
-        <v>142</v>
-      </c>
-      <c r="D6" t="s">
-        <v>113</v>
-      </c>
-      <c r="E6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F6">
-        <v>234567891</v>
-      </c>
-      <c r="G6" s="1">
-        <v>2</v>
-      </c>
-      <c r="H6" t="s">
-        <v>122</v>
-      </c>
-      <c r="I6" t="s">
-        <v>113</v>
-      </c>
-      <c r="J6" t="s">
-        <v>113</v>
-      </c>
-      <c r="K6" t="s">
-        <v>121</v>
-      </c>
-      <c r="L6" t="s">
-        <v>190</v>
-      </c>
-      <c r="M6">
-        <v>99999</v>
-      </c>
-      <c r="N6">
-        <v>1</v>
-      </c>
-      <c r="P6" t="str">
-        <f>$P$1&amp;B6&amp;",'"&amp;C6&amp;"',"&amp;IF(D6="NULL","NULL,'","'"&amp;D6&amp;"','")&amp;E6&amp;"',"&amp;F6&amp;",'"&amp;TEXT(G6,("yyyy-mm-dd"))&amp;"','"&amp;H6&amp;"',"&amp;I6&amp;","&amp;J6&amp;",'"&amp;K6&amp;"','"&amp;L6&amp;"','"&amp;M6&amp;"',"&amp;N6</f>
-        <v>EXEC cust.SP_InsertInsureesAccountData NULL,'Sharon',NULL,'Paesachov',234567891,'1900-01-02','124 Awesome street',NULL,NULL,'Anytown','CA','99999',1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <f t="shared" ref="A7:A25" si="0">A6+1</f>
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>113</v>
-      </c>
-      <c r="C7" t="s">
-        <v>145</v>
-      </c>
-      <c r="D7" t="s">
-        <v>113</v>
-      </c>
-      <c r="E7" t="s">
-        <v>144</v>
-      </c>
-      <c r="F7">
-        <v>123456791</v>
-      </c>
-      <c r="G7" s="1">
-        <v>3</v>
-      </c>
-      <c r="H7" t="s">
-        <v>123</v>
-      </c>
-      <c r="I7" t="s">
-        <v>113</v>
-      </c>
-      <c r="J7" t="s">
-        <v>113</v>
-      </c>
-      <c r="K7" t="s">
-        <v>188</v>
-      </c>
-      <c r="L7" t="s">
-        <v>190</v>
-      </c>
-      <c r="M7">
-        <v>99999</v>
-      </c>
-      <c r="N7">
-        <v>1</v>
-      </c>
-      <c r="P7" t="str">
-        <f t="shared" ref="P7:P25" si="1">$P$1&amp;B7&amp;",'"&amp;C7&amp;"',"&amp;IF(D7="NULL","NULL,'","'"&amp;D7&amp;"','")&amp;E7&amp;"',"&amp;F7&amp;",'"&amp;TEXT(G7,("yyyy-mm-dd"))&amp;"','"&amp;H7&amp;"',"&amp;I7&amp;","&amp;J7&amp;",'"&amp;K7&amp;"','"&amp;L7&amp;"','"&amp;M7&amp;"',"&amp;N7</f>
-        <v>EXEC cust.SP_InsertInsureesAccountData NULL,'Anomandaris',NULL,'Dragnipurake',123456791,'1900-01-03','125 Awesome street',NULL,NULL,'Kurald Galain','CA','99999',1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>113</v>
-      </c>
-      <c r="C8" t="s">
-        <v>146</v>
-      </c>
-      <c r="D8" t="s">
-        <v>147</v>
-      </c>
-      <c r="E8" t="s">
-        <v>148</v>
-      </c>
-      <c r="F8">
-        <v>123456792</v>
-      </c>
-      <c r="G8" s="1">
-        <v>4</v>
-      </c>
-      <c r="H8" t="s">
-        <v>124</v>
-      </c>
-      <c r="I8" t="s">
-        <v>113</v>
-      </c>
-      <c r="J8" t="s">
-        <v>113</v>
-      </c>
-      <c r="K8" t="s">
-        <v>189</v>
-      </c>
-      <c r="L8" t="s">
-        <v>191</v>
-      </c>
-      <c r="M8">
-        <v>99999</v>
-      </c>
-      <c r="N8">
-        <v>1</v>
-      </c>
-      <c r="P8" t="str">
-        <f t="shared" si="1"/>
-        <v>EXEC cust.SP_InsertInsureesAccountData NULL,'Butt','Face','McPoopypants',123456792,'1900-01-04','126 Awesome street',NULL,NULL,'Poopsville','NV','99999',1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B9" t="s">
-        <v>113</v>
-      </c>
-      <c r="C9" t="s">
-        <v>149</v>
-      </c>
-      <c r="D9" t="s">
-        <v>113</v>
-      </c>
-      <c r="E9" t="s">
-        <v>150</v>
-      </c>
-      <c r="F9">
-        <v>123456793</v>
-      </c>
-      <c r="G9" s="1">
-        <v>5</v>
-      </c>
-      <c r="H9" t="s">
-        <v>125</v>
-      </c>
-      <c r="I9" t="s">
-        <v>113</v>
-      </c>
-      <c r="J9" t="s">
-        <v>113</v>
-      </c>
-      <c r="K9" t="s">
-        <v>192</v>
-      </c>
-      <c r="L9" t="s">
-        <v>190</v>
-      </c>
-      <c r="M9">
-        <v>99999</v>
-      </c>
-      <c r="N9">
-        <v>1</v>
-      </c>
-      <c r="P9" t="str">
-        <f t="shared" si="1"/>
-        <v>EXEC cust.SP_InsertInsureesAccountData NULL,'Trull',NULL,'Sengar',123456793,'1900-01-05','127 Awesome street',NULL,NULL,'Kurald Emurhlan','CA','99999',1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B10" t="s">
-        <v>113</v>
-      </c>
-      <c r="C10" t="s">
-        <v>151</v>
-      </c>
-      <c r="D10" t="s">
-        <v>113</v>
-      </c>
-      <c r="E10" t="s">
-        <v>152</v>
-      </c>
-      <c r="F10">
-        <v>123456794</v>
-      </c>
-      <c r="G10" s="1">
-        <v>6</v>
-      </c>
-      <c r="H10" t="s">
-        <v>126</v>
-      </c>
-      <c r="I10" t="s">
-        <v>113</v>
-      </c>
-      <c r="J10" t="s">
-        <v>113</v>
-      </c>
-      <c r="K10" t="s">
-        <v>203</v>
-      </c>
-      <c r="L10" t="s">
-        <v>190</v>
-      </c>
-      <c r="M10">
-        <v>99999</v>
-      </c>
-      <c r="N10">
-        <v>1</v>
-      </c>
-      <c r="P10" t="str">
-        <f t="shared" si="1"/>
-        <v>EXEC cust.SP_InsertInsureesAccountData NULL,'Paul',NULL,'Atreides',123456794,'1900-01-06','128 Awesome street',NULL,NULL,'Caladan','CA','99999',1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B11" t="s">
-        <v>113</v>
-      </c>
-      <c r="C11" t="s">
-        <v>153</v>
-      </c>
-      <c r="D11" t="s">
-        <v>113</v>
-      </c>
-      <c r="E11" t="s">
-        <v>154</v>
-      </c>
-      <c r="F11">
-        <v>123456795</v>
-      </c>
-      <c r="G11" s="1">
-        <v>7</v>
-      </c>
-      <c r="H11" t="s">
-        <v>127</v>
-      </c>
-      <c r="I11" t="s">
-        <v>113</v>
-      </c>
-      <c r="J11" t="s">
-        <v>113</v>
-      </c>
-      <c r="K11" t="s">
-        <v>194</v>
-      </c>
-      <c r="L11" t="s">
-        <v>190</v>
-      </c>
-      <c r="M11">
-        <v>99999</v>
-      </c>
-      <c r="N11">
-        <v>1</v>
-      </c>
-      <c r="P11" t="str">
-        <f t="shared" si="1"/>
-        <v>EXEC cust.SP_InsertInsureesAccountData NULL,'Karsa',NULL,'Orlong',123456795,'1900-01-07','129 Awesome street',NULL,NULL,'Teblor','CA','99999',1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B12" t="s">
-        <v>113</v>
-      </c>
-      <c r="C12" t="s">
-        <v>155</v>
-      </c>
-      <c r="D12" t="s">
-        <v>113</v>
-      </c>
-      <c r="E12" t="s">
-        <v>156</v>
-      </c>
-      <c r="F12">
-        <v>123456796</v>
-      </c>
-      <c r="G12" s="1">
-        <v>8</v>
-      </c>
-      <c r="H12" t="s">
-        <v>128</v>
-      </c>
-      <c r="I12" t="s">
-        <v>113</v>
-      </c>
-      <c r="J12" t="s">
-        <v>113</v>
-      </c>
-      <c r="K12" t="s">
-        <v>195</v>
-      </c>
-      <c r="L12" t="s">
-        <v>190</v>
-      </c>
-      <c r="M12">
-        <v>99999</v>
-      </c>
-      <c r="N12">
-        <v>1</v>
-      </c>
-      <c r="P12" t="str">
-        <f t="shared" si="1"/>
-        <v>EXEC cust.SP_InsertInsureesAccountData NULL,'Whiskey',NULL,'Jack',123456796,'1900-01-08','130 Awesome street',NULL,NULL,'Malazan','CA','99999',1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B13" t="s">
-        <v>113</v>
-      </c>
-      <c r="C13" t="s">
-        <v>157</v>
-      </c>
-      <c r="D13" t="s">
-        <v>113</v>
-      </c>
-      <c r="E13" t="s">
-        <v>158</v>
-      </c>
-      <c r="F13">
-        <v>123456797</v>
-      </c>
-      <c r="G13" s="1">
-        <v>9</v>
-      </c>
-      <c r="H13" t="s">
-        <v>129</v>
-      </c>
-      <c r="I13" t="s">
-        <v>113</v>
-      </c>
-      <c r="J13" t="s">
-        <v>113</v>
-      </c>
-      <c r="K13" t="s">
-        <v>195</v>
-      </c>
-      <c r="L13" t="s">
-        <v>190</v>
-      </c>
-      <c r="M13">
-        <v>99999</v>
-      </c>
-      <c r="N13">
-        <v>1</v>
-      </c>
-      <c r="P13" t="str">
-        <f t="shared" si="1"/>
-        <v>EXEC cust.SP_InsertInsureesAccountData NULL,'Fiddler',NULL,'Strings',123456797,'1900-01-09','131 Awesome street',NULL,NULL,'Malazan','CA','99999',1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B14" t="s">
-        <v>113</v>
-      </c>
-      <c r="C14" t="s">
-        <v>160</v>
-      </c>
-      <c r="D14" t="s">
-        <v>159</v>
-      </c>
-      <c r="E14" t="s">
-        <v>161</v>
-      </c>
-      <c r="F14">
-        <v>123456798</v>
-      </c>
-      <c r="G14" s="1">
-        <v>10</v>
-      </c>
-      <c r="H14" t="s">
-        <v>130</v>
-      </c>
-      <c r="I14" t="s">
-        <v>113</v>
-      </c>
-      <c r="J14" t="s">
-        <v>113</v>
-      </c>
-      <c r="K14" t="s">
-        <v>196</v>
-      </c>
-      <c r="L14" t="s">
-        <v>197</v>
-      </c>
-      <c r="M14">
-        <v>99999</v>
-      </c>
-      <c r="N14">
-        <v>1</v>
-      </c>
-      <c r="P14" t="str">
-        <f t="shared" si="1"/>
-        <v>EXEC cust.SP_InsertInsureesAccountData NULL,'Clark','Superman','Kent',123456798,'1900-01-10','132 Awesome street',NULL,NULL,'Smallville','IO','99999',1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B15" t="s">
-        <v>113</v>
-      </c>
-      <c r="C15" t="s">
-        <v>162</v>
-      </c>
-      <c r="D15" t="s">
-        <v>163</v>
-      </c>
-      <c r="E15" t="s">
-        <v>164</v>
-      </c>
-      <c r="F15">
-        <v>123456799</v>
-      </c>
-      <c r="G15" s="1">
-        <v>11</v>
-      </c>
-      <c r="H15" t="s">
-        <v>131</v>
-      </c>
-      <c r="I15" t="s">
-        <v>113</v>
-      </c>
-      <c r="J15" t="s">
-        <v>113</v>
-      </c>
-      <c r="K15" t="s">
-        <v>198</v>
-      </c>
-      <c r="L15" t="s">
-        <v>199</v>
-      </c>
-      <c r="M15">
-        <v>99999</v>
-      </c>
-      <c r="N15">
-        <v>1</v>
-      </c>
-      <c r="P15" t="str">
-        <f t="shared" si="1"/>
-        <v>EXEC cust.SP_InsertInsureesAccountData NULL,'Bruce','Batman','Wayne',123456799,'1900-01-11','133 Awesome street',NULL,NULL,'Gotham City','NY','99999',1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="B16" t="s">
-        <v>113</v>
-      </c>
-      <c r="C16" t="s">
-        <v>165</v>
-      </c>
-      <c r="D16" t="s">
-        <v>113</v>
-      </c>
-      <c r="E16" t="s">
-        <v>166</v>
-      </c>
-      <c r="F16">
-        <v>123456800</v>
-      </c>
-      <c r="G16" s="1">
-        <v>12</v>
-      </c>
-      <c r="H16" t="s">
-        <v>132</v>
-      </c>
-      <c r="I16" t="s">
-        <v>113</v>
-      </c>
-      <c r="J16" t="s">
-        <v>113</v>
-      </c>
-      <c r="K16" t="s">
-        <v>195</v>
-      </c>
-      <c r="L16" t="s">
-        <v>190</v>
-      </c>
-      <c r="M16">
-        <v>99999</v>
-      </c>
-      <c r="N16">
-        <v>1</v>
-      </c>
-      <c r="P16" t="str">
-        <f t="shared" si="1"/>
-        <v>EXEC cust.SP_InsertInsureesAccountData NULL,'Dassem',NULL,'Ultor',123456800,'1900-01-12','134 Awesome street',NULL,NULL,'Malazan','CA','99999',1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="B17" t="s">
-        <v>113</v>
-      </c>
-      <c r="C17" t="s">
-        <v>167</v>
-      </c>
-      <c r="D17" t="s">
-        <v>169</v>
-      </c>
-      <c r="E17" t="s">
-        <v>168</v>
-      </c>
-      <c r="F17">
-        <v>123456801</v>
-      </c>
-      <c r="G17" s="1">
-        <v>13</v>
-      </c>
-      <c r="H17" t="s">
-        <v>133</v>
-      </c>
-      <c r="I17" t="s">
-        <v>113</v>
-      </c>
-      <c r="J17" t="s">
-        <v>113</v>
-      </c>
-      <c r="K17" t="s">
-        <v>200</v>
-      </c>
-      <c r="L17" t="s">
-        <v>190</v>
-      </c>
-      <c r="M17">
-        <v>99999</v>
-      </c>
-      <c r="N17">
-        <v>1</v>
-      </c>
-      <c r="P17" t="str">
-        <f t="shared" si="1"/>
-        <v>EXEC cust.SP_InsertInsureesAccountData NULL,'Onos','FirstSword','T'oolan',123456801,'1900-01-13','135 Awesome street',NULL,NULL,'Clanless','CA','99999',1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="B18" t="s">
-        <v>113</v>
-      </c>
-      <c r="C18" t="s">
-        <v>170</v>
-      </c>
-      <c r="D18" t="s">
-        <v>113</v>
-      </c>
-      <c r="E18" t="s">
-        <v>171</v>
-      </c>
-      <c r="F18">
-        <v>123456802</v>
-      </c>
-      <c r="G18" s="1">
-        <v>14</v>
-      </c>
-      <c r="H18" t="s">
-        <v>134</v>
-      </c>
-      <c r="I18" t="s">
-        <v>113</v>
-      </c>
-      <c r="J18" t="s">
-        <v>113</v>
-      </c>
-      <c r="K18" t="s">
-        <v>195</v>
-      </c>
-      <c r="L18" t="s">
-        <v>190</v>
-      </c>
-      <c r="M18">
-        <v>99999</v>
-      </c>
-      <c r="N18">
-        <v>1</v>
-      </c>
-      <c r="P18" t="str">
-        <f t="shared" si="1"/>
-        <v>EXEC cust.SP_InsertInsureesAccountData NULL,'Kalam',NULL,'Mekhar',123456802,'1900-01-14','136 Awesome street',NULL,NULL,'Malazan','CA','99999',1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="B19" t="s">
-        <v>113</v>
-      </c>
-      <c r="C19" t="s">
-        <v>172</v>
-      </c>
-      <c r="D19" t="s">
-        <v>173</v>
-      </c>
-      <c r="E19" t="s">
-        <v>174</v>
-      </c>
-      <c r="F19">
-        <v>123456803</v>
-      </c>
-      <c r="G19" s="1">
-        <v>15</v>
-      </c>
-      <c r="H19" t="s">
-        <v>135</v>
-      </c>
-      <c r="I19" t="s">
-        <v>113</v>
-      </c>
-      <c r="J19" t="s">
-        <v>113</v>
-      </c>
-      <c r="K19" t="s">
-        <v>201</v>
-      </c>
-      <c r="L19" t="s">
-        <v>190</v>
-      </c>
-      <c r="M19">
-        <v>99999</v>
-      </c>
-      <c r="N19">
-        <v>1</v>
-      </c>
-      <c r="P19" t="str">
-        <f t="shared" si="1"/>
-        <v>EXEC cust.SP_InsertInsureesAccountData NULL,'Eye','See','Youpee',123456803,'1900-01-15','137 Awesome street',NULL,NULL,'Somewhere Gross','CA','99999',1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="B20" t="s">
-        <v>113</v>
-      </c>
-      <c r="C20" t="s">
-        <v>175</v>
-      </c>
-      <c r="D20" t="s">
-        <v>113</v>
-      </c>
-      <c r="E20" t="s">
-        <v>176</v>
-      </c>
-      <c r="F20">
-        <v>123456804</v>
-      </c>
-      <c r="G20" s="1">
-        <v>16</v>
-      </c>
-      <c r="H20" t="s">
-        <v>136</v>
-      </c>
-      <c r="I20" t="s">
-        <v>113</v>
-      </c>
-      <c r="J20" t="s">
-        <v>113</v>
-      </c>
-      <c r="K20" t="s">
-        <v>202</v>
-      </c>
-      <c r="L20" t="s">
-        <v>190</v>
-      </c>
-      <c r="M20">
-        <v>99999</v>
-      </c>
-      <c r="N20">
-        <v>1</v>
-      </c>
-      <c r="P20" t="str">
-        <f t="shared" si="1"/>
-        <v>EXEC cust.SP_InsertInsureesAccountData NULL,'Elephant',NULL,'Shoe',123456804,'1900-01-16','138 Awesome street',NULL,NULL,'La Zoo','CA','99999',1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="B21" t="s">
-        <v>113</v>
-      </c>
-      <c r="C21" t="s">
-        <v>177</v>
-      </c>
-      <c r="D21" t="s">
-        <v>113</v>
-      </c>
-      <c r="E21" t="s">
-        <v>178</v>
-      </c>
-      <c r="F21">
-        <v>123456805</v>
-      </c>
-      <c r="G21" s="1">
-        <v>17</v>
-      </c>
-      <c r="H21" t="s">
-        <v>137</v>
-      </c>
-      <c r="I21" t="s">
-        <v>113</v>
-      </c>
-      <c r="J21" t="s">
-        <v>113</v>
-      </c>
-      <c r="K21" t="s">
-        <v>121</v>
-      </c>
-      <c r="L21" t="s">
-        <v>190</v>
-      </c>
-      <c r="M21">
-        <v>99999</v>
-      </c>
-      <c r="N21">
-        <v>1</v>
-      </c>
-      <c r="P21" t="str">
-        <f t="shared" si="1"/>
-        <v>EXEC cust.SP_InsertInsureesAccountData NULL,'Kurt',NULL,'Vonnegut',123456805,'1900-01-17','139 Awesome street',NULL,NULL,'Anytown','CA','99999',1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="B22" t="s">
-        <v>113</v>
-      </c>
-      <c r="C22" t="s">
-        <v>179</v>
-      </c>
-      <c r="D22" t="s">
-        <v>113</v>
-      </c>
-      <c r="E22" t="s">
-        <v>180</v>
-      </c>
-      <c r="F22">
-        <v>123456806</v>
-      </c>
-      <c r="G22" s="1">
-        <v>18</v>
-      </c>
-      <c r="H22" t="s">
-        <v>138</v>
-      </c>
-      <c r="I22" t="s">
-        <v>113</v>
-      </c>
-      <c r="J22" t="s">
-        <v>113</v>
-      </c>
-      <c r="K22" t="s">
-        <v>193</v>
-      </c>
-      <c r="L22" t="s">
-        <v>190</v>
-      </c>
-      <c r="M22">
-        <v>99999</v>
-      </c>
-      <c r="N22">
-        <v>1</v>
-      </c>
-      <c r="P22" t="str">
-        <f t="shared" si="1"/>
-        <v>EXEC cust.SP_InsertInsureesAccountData NULL,'Muad',NULL,'Dib',123456806,'1900-01-18','140 Awesome street',NULL,NULL,'Dune','CA','99999',1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="B23" t="s">
-        <v>113</v>
-      </c>
-      <c r="C23" t="s">
-        <v>181</v>
-      </c>
-      <c r="D23" t="s">
-        <v>182</v>
-      </c>
-      <c r="E23" t="s">
-        <v>183</v>
-      </c>
-      <c r="F23">
-        <v>123456807</v>
-      </c>
-      <c r="G23" s="1">
-        <v>19</v>
-      </c>
-      <c r="H23" t="s">
-        <v>139</v>
-      </c>
-      <c r="I23" t="s">
-        <v>113</v>
-      </c>
-      <c r="J23" t="s">
-        <v>113</v>
-      </c>
-      <c r="K23" t="s">
-        <v>204</v>
-      </c>
-      <c r="L23" t="s">
-        <v>190</v>
-      </c>
-      <c r="M23">
-        <v>99999</v>
-      </c>
-      <c r="N23">
-        <v>1</v>
-      </c>
-      <c r="P23" t="str">
-        <f t="shared" si="1"/>
-        <v>EXEC cust.SP_InsertInsureesAccountData NULL,'Mario','And','Luigi',123456807,'1900-01-19','141 Awesome street',NULL,NULL,'Nintendo','CA','99999',1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="B24" t="s">
-        <v>113</v>
-      </c>
-      <c r="C24" t="s">
-        <v>184</v>
-      </c>
-      <c r="D24" t="s">
-        <v>113</v>
-      </c>
-      <c r="E24" t="s">
-        <v>185</v>
-      </c>
-      <c r="F24">
-        <v>123456808</v>
-      </c>
-      <c r="G24" s="1">
-        <v>20</v>
-      </c>
-      <c r="H24" t="s">
-        <v>140</v>
-      </c>
-      <c r="I24" t="s">
-        <v>113</v>
-      </c>
-      <c r="J24" t="s">
-        <v>113</v>
-      </c>
-      <c r="K24" t="s">
-        <v>204</v>
-      </c>
-      <c r="L24" t="s">
-        <v>190</v>
-      </c>
-      <c r="M24">
-        <v>99999</v>
-      </c>
-      <c r="N24">
-        <v>1</v>
-      </c>
-      <c r="P24" t="str">
-        <f t="shared" si="1"/>
-        <v>EXEC cust.SP_InsertInsureesAccountData NULL,'Princess',NULL,'Peach',123456808,'1900-01-20','142 Awesome street',NULL,NULL,'Nintendo','CA','99999',1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="B25" t="s">
-        <v>113</v>
-      </c>
-      <c r="C25" t="s">
-        <v>186</v>
-      </c>
-      <c r="D25" t="s">
-        <v>113</v>
-      </c>
-      <c r="E25" t="s">
-        <v>187</v>
-      </c>
-      <c r="F25">
-        <v>123456809</v>
-      </c>
-      <c r="G25" s="1">
-        <v>21</v>
-      </c>
-      <c r="H25" t="s">
-        <v>141</v>
-      </c>
-      <c r="I25" t="s">
-        <v>113</v>
-      </c>
-      <c r="J25" t="s">
-        <v>113</v>
-      </c>
-      <c r="K25" t="s">
-        <v>204</v>
-      </c>
-      <c r="L25" t="s">
-        <v>190</v>
-      </c>
-      <c r="M25">
-        <v>99999</v>
-      </c>
-      <c r="N25">
-        <v>1</v>
-      </c>
-      <c r="P25" t="str">
-        <f t="shared" si="1"/>
-        <v>EXEC cust.SP_InsertInsureesAccountData NULL,'King ',NULL,'Koopa',123456809,'1900-01-21','143 Awesome street',NULL,NULL,'Nintendo','CA','99999',1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>206</v>
-      </c>
-      <c r="B28" t="s">
-        <v>207</v>
-      </c>
-      <c r="C28" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>206</v>
-      </c>
-      <c r="B29" t="s">
-        <v>257</v>
-      </c>
-      <c r="C29" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>206</v>
-      </c>
-      <c r="B30" t="s">
-        <v>259</v>
-      </c>
-      <c r="C30" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>206</v>
-      </c>
-      <c r="B31" t="s">
-        <v>208</v>
-      </c>
-      <c r="C31" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>206</v>
-      </c>
-      <c r="B32" t="s">
-        <v>260</v>
-      </c>
-      <c r="C32" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>206</v>
-      </c>
-      <c r="B33" t="s">
-        <v>261</v>
-      </c>
-      <c r="C33" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>206</v>
-      </c>
-      <c r="B34" t="s">
-        <v>209</v>
-      </c>
-      <c r="C34" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>206</v>
-      </c>
-      <c r="B35" t="s">
-        <v>262</v>
-      </c>
-      <c r="C35" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>206</v>
-      </c>
-      <c r="B36" t="s">
-        <v>210</v>
-      </c>
-      <c r="C36" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>206</v>
-      </c>
-      <c r="B37" t="s">
-        <v>263</v>
-      </c>
-      <c r="C37" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>206</v>
-      </c>
-      <c r="B38" t="s">
-        <v>211</v>
-      </c>
-      <c r="C38" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>206</v>
-      </c>
-      <c r="B39" t="s">
-        <v>264</v>
-      </c>
-      <c r="C39" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>206</v>
-      </c>
-      <c r="B40" t="s">
-        <v>212</v>
-      </c>
-      <c r="C40" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>206</v>
-      </c>
-      <c r="B41" t="s">
-        <v>213</v>
-      </c>
-      <c r="C41" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>206</v>
-      </c>
-      <c r="B42" t="s">
-        <v>214</v>
-      </c>
-      <c r="C42" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>206</v>
-      </c>
-      <c r="B43" t="s">
-        <v>215</v>
-      </c>
-      <c r="C43" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>206</v>
-      </c>
-      <c r="B44" t="s">
-        <v>216</v>
-      </c>
-      <c r="C44" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>206</v>
-      </c>
-      <c r="B45" t="s">
-        <v>217</v>
-      </c>
-      <c r="C45" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>206</v>
-      </c>
-      <c r="B46" t="s">
-        <v>218</v>
-      </c>
-      <c r="C46" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>206</v>
-      </c>
-      <c r="B47" t="s">
-        <v>219</v>
-      </c>
-      <c r="C47" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>206</v>
-      </c>
-      <c r="B48" t="s">
-        <v>220</v>
-      </c>
-      <c r="C48" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>206</v>
-      </c>
-      <c r="B49" t="s">
-        <v>221</v>
-      </c>
-      <c r="C49" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>206</v>
-      </c>
-      <c r="B50" t="s">
-        <v>222</v>
-      </c>
-      <c r="C50" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>206</v>
-      </c>
-      <c r="B51" t="s">
-        <v>223</v>
-      </c>
-      <c r="C51" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>206</v>
-      </c>
-      <c r="B52" t="s">
-        <v>224</v>
-      </c>
-      <c r="C52" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>206</v>
-      </c>
-      <c r="B53" t="s">
-        <v>225</v>
-      </c>
-      <c r="C53" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>206</v>
-      </c>
-      <c r="B54" t="s">
-        <v>226</v>
-      </c>
-      <c r="C54" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>206</v>
-      </c>
-      <c r="B55" t="s">
-        <v>227</v>
-      </c>
-      <c r="C55" t="s">
-        <v>256</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D569725A-CFCB-4C23-8C05-40AC3BB952B1}">
-  <dimension ref="A1:J16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H1" t="s">
-        <v>232</v>
-      </c>
-      <c r="I1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J1" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>232</v>
-      </c>
-      <c r="B2" t="s">
-        <v>233</v>
-      </c>
-      <c r="C2" t="s">
-        <v>234</v>
-      </c>
-      <c r="D2">
-        <v>4</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
-        <v>240</v>
-      </c>
-      <c r="J2" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>235</v>
-      </c>
-      <c r="B3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C3" t="s">
-        <v>234</v>
-      </c>
-      <c r="D3">
-        <v>8</v>
-      </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
-      <c r="I3" t="s">
-        <v>242</v>
-      </c>
-      <c r="J3" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>236</v>
-      </c>
-      <c r="B4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C4" t="s">
-        <v>234</v>
-      </c>
-      <c r="D4">
-        <v>25</v>
-      </c>
-      <c r="H4">
-        <v>3</v>
-      </c>
-      <c r="I4" t="s">
-        <v>244</v>
-      </c>
-      <c r="J4" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>237</v>
-      </c>
-      <c r="B5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C5" t="s">
-        <v>234</v>
-      </c>
-      <c r="D5">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>238</v>
-      </c>
-      <c r="B6" t="s">
-        <v>233</v>
-      </c>
-      <c r="C6" t="s">
-        <v>234</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-      <c r="H6" t="s">
-        <v>232</v>
-      </c>
-      <c r="I6" t="s">
-        <v>27</v>
-      </c>
-      <c r="J6" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>239</v>
-      </c>
-      <c r="B7" t="s">
-        <v>233</v>
-      </c>
-      <c r="C7" t="s">
-        <v>234</v>
-      </c>
-      <c r="D7">
-        <v>4</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7" t="s">
-        <v>247</v>
-      </c>
-      <c r="J7" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H8">
-        <v>2</v>
-      </c>
-      <c r="I8" t="s">
-        <v>248</v>
-      </c>
-      <c r="J8" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H9">
-        <v>3</v>
-      </c>
-      <c r="I9" t="s">
-        <v>249</v>
-      </c>
-      <c r="J9" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>232</v>
-      </c>
-      <c r="B10" t="s">
-        <v>233</v>
-      </c>
-      <c r="C10" t="s">
-        <v>234</v>
-      </c>
-      <c r="D10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>235</v>
-      </c>
-      <c r="B11" t="s">
-        <v>104</v>
-      </c>
-      <c r="C11" t="s">
-        <v>234</v>
-      </c>
-      <c r="D11">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>236</v>
-      </c>
-      <c r="B12" t="s">
-        <v>97</v>
-      </c>
-      <c r="C12" t="s">
-        <v>234</v>
-      </c>
-      <c r="D12">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" t="s">
-        <v>97</v>
-      </c>
-      <c r="C13" t="s">
-        <v>234</v>
-      </c>
-      <c r="D13">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>250</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Completed all fake data inserts
</commit_message>
<xml_diff>
--- a/Database Repository/EdusafeServicingDB Repository/0. Helper Scripts and Excel/Helper Workbook.xlsx
+++ b/Database Repository/EdusafeServicingDB Repository/0. Helper Scripts and Excel/Helper Workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dar Vadar\Desktop\EduSafe Repo\edusafe\Database Repository\EdusafeServicingDB Repository\0. Helper Scripts and Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{645275E1-67CD-42C8-BC59-BBBC54C842AE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEEC5EF3-BB6A-4434-A0DA-59008F5ACB78}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4F07375E-5034-49E5-AD40-EDFCB413E4AD}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{4F07375E-5034-49E5-AD40-EDFCB413E4AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Entries" sheetId="2" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="102">
   <si>
     <t>Database</t>
   </si>
@@ -808,7 +808,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D6E4056-ECB1-45E1-9DAC-970AA7C8F4F6}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
@@ -1462,8 +1462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF7A6780-4CB8-4C87-9527-D541C7D9DA48}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2087,8 +2087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{746F0001-40B4-4DDF-A81A-84108DB4EF26}">
   <dimension ref="A1:C73"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38:C39"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2954,12 +2954,57 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B336A336-1BB4-460C-BDA2-63E68686386A}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" t="str">
+        <f t="shared" ref="D2" si="0">"sqlcmd -S "
+&amp;Entries_Server
+&amp;" -d "
+&amp;Entries_Database
+&amp;" -U "
+&amp;Entries_User
+&amp;" -P "
+&amp;Entries_Password
+&amp;" -i "
+&amp;Entries_StoredProcedure_RootPath
+&amp;B2&amp;A2&amp;C2
+&amp;""""
+&amp;" &gt;&gt; """
+&amp;Entries_StoredProcedure_DebugText</f>
+        <v>sqlcmd -S edusafe.database.windows.net  -d EdusafeServicingDB -U EduSafeAdmin -P Master123 -i "2. Stored Procedures\cust.SP_DeleteEmails.StoredProcedure.sql" &gt;&gt; "CreateSp.txt</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>